<commit_message>
UI tomoni uchun qilingan o'zgarishlar
</commit_message>
<xml_diff>
--- a/xisobot.xlsx
+++ b/xisobot.xlsx
@@ -481,15 +481,15 @@
         <v>160000</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-04-19</t>
+          <t>2022-04-22</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>640000</v>
+        <v>160000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>